<commit_message>
updated examples and input excel files
</commit_message>
<xml_diff>
--- a/Example input/Kansas/kansas inputs.xlsx
+++ b/Example input/Kansas/kansas inputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9B1C44-B37E-4174-8CEF-FF547F2E9AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2283CF0A-204F-4581-A05F-2ACF2463BF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4176" yWindow="2484" windowWidth="15168" windowHeight="7536" tabRatio="824" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="852" windowWidth="17988" windowHeight="11652" tabRatio="824" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="5" r:id="rId1"/>
@@ -1733,25 +1733,25 @@
       <selection activeCell="S1" sqref="S1:V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.3515625" customWidth="1"/>
-    <col min="3" max="3" width="17.1171875" customWidth="1"/>
-    <col min="4" max="5" width="19.1171875" customWidth="1"/>
-    <col min="6" max="6" width="16.1171875" customWidth="1"/>
-    <col min="7" max="7" width="21.41015625" customWidth="1"/>
+    <col min="1" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="19.1171875" customWidth="1"/>
-    <col min="10" max="10" width="12.41015625" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="18.1171875" customWidth="1"/>
-    <col min="14" max="14" width="14.1171875" customWidth="1"/>
-    <col min="15" max="15" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.76171875" customWidth="1"/>
-    <col min="19" max="21" width="17.41015625" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.77734375" customWidth="1"/>
+    <col min="19" max="21" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -2463,22 +2463,22 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.3515625" customWidth="1"/>
-    <col min="3" max="3" width="8.3515625" customWidth="1"/>
-    <col min="6" max="6" width="11.3515625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.64453125" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="13.87890625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="9.64453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.1171875" style="10"/>
-    <col min="16" max="16" width="14.1171875" style="10" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" style="10" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.109375" style="10"/>
+    <col min="16" max="16" width="14.109375" style="10" customWidth="1"/>
     <col min="17" max="17" width="14" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -3109,23 +3109,23 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AR213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <pane ySplit="600" activePane="bottomLeft"/>
       <selection activeCell="E2" sqref="E1:E1048576"/>
       <selection pane="bottomLeft" activeCell="P2" sqref="P2:P213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.52734375" customWidth="1"/>
-    <col min="2" max="11" width="14.64453125" customWidth="1"/>
-    <col min="12" max="12" width="7.3515625" customWidth="1"/>
-    <col min="13" max="13" width="11.52734375" customWidth="1"/>
-    <col min="14" max="22" width="14.64453125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="22" width="14.6640625" customWidth="1"/>
     <col min="23" max="31" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>222</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -6341,7 +6341,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -7413,7 +7413,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
@@ -7547,7 +7547,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>28</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>28</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>29</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>29</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>29</v>
       </c>
@@ -8485,7 +8485,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>29</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>29</v>
       </c>
@@ -8753,7 +8753,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>29</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="44" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>173</v>
       </c>
@@ -9021,7 +9021,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="45" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>173</v>
       </c>
@@ -9155,7 +9155,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>173</v>
       </c>
@@ -9289,7 +9289,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="47" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>173</v>
       </c>
@@ -9423,7 +9423,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>173</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>173</v>
       </c>
@@ -9691,7 +9691,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="50" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>173</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>173</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>174</v>
       </c>
@@ -10093,7 +10093,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>174</v>
       </c>
@@ -10227,7 +10227,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>174</v>
       </c>
@@ -10361,7 +10361,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="55" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>174</v>
       </c>
@@ -10495,7 +10495,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>174</v>
       </c>
@@ -10629,7 +10629,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>174</v>
       </c>
@@ -10763,7 +10763,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="58" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>174</v>
       </c>
@@ -10897,7 +10897,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="59" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>174</v>
       </c>
@@ -11031,7 +11031,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="E60">
         <v>-1</v>
@@ -11091,7 +11091,7 @@
       <c r="AJ60" s="13"/>
       <c r="AR60" s="13"/>
     </row>
-    <row r="61" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="E61">
         <v>-1</v>
@@ -11151,7 +11151,7 @@
       <c r="AJ61" s="13"/>
       <c r="AR61" s="13"/>
     </row>
-    <row r="62" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="E62">
         <v>-1</v>
@@ -11211,7 +11211,7 @@
       <c r="AJ62" s="13"/>
       <c r="AR62" s="13"/>
     </row>
-    <row r="63" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="E63">
         <v>-1</v>
@@ -11271,7 +11271,7 @@
       <c r="AJ63" s="13"/>
       <c r="AR63" s="13"/>
     </row>
-    <row r="64" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="E64">
         <v>-1</v>
@@ -11331,7 +11331,7 @@
       <c r="AJ64" s="13"/>
       <c r="AR64" s="13"/>
     </row>
-    <row r="65" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="E65">
         <v>-1</v>
@@ -11391,7 +11391,7 @@
       <c r="AJ65" s="13"/>
       <c r="AR65" s="13"/>
     </row>
-    <row r="66" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="E66">
         <v>-1</v>
@@ -11451,7 +11451,7 @@
       <c r="AJ66" s="13"/>
       <c r="AR66" s="13"/>
     </row>
-    <row r="67" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="E67">
         <v>-1</v>
@@ -11511,7 +11511,7 @@
       <c r="AJ67" s="13"/>
       <c r="AR67" s="13"/>
     </row>
-    <row r="68" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="E68">
         <v>-1</v>
@@ -11571,7 +11571,7 @@
       <c r="AJ68" s="13"/>
       <c r="AR68" s="13"/>
     </row>
-    <row r="69" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="E69">
         <v>-1</v>
@@ -11631,7 +11631,7 @@
       <c r="AJ69" s="13"/>
       <c r="AR69" s="13"/>
     </row>
-    <row r="70" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="E70">
         <v>-1</v>
@@ -11691,7 +11691,7 @@
       <c r="AJ70" s="13"/>
       <c r="AR70" s="13"/>
     </row>
-    <row r="71" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="E71">
         <v>-1</v>
@@ -11751,7 +11751,7 @@
       <c r="AJ71" s="13"/>
       <c r="AR71" s="13"/>
     </row>
-    <row r="72" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="E72">
         <v>-1</v>
@@ -11811,7 +11811,7 @@
       <c r="AJ72" s="13"/>
       <c r="AR72" s="13"/>
     </row>
-    <row r="73" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="E73">
         <v>-1</v>
@@ -11871,7 +11871,7 @@
       <c r="AJ73" s="13"/>
       <c r="AR73" s="13"/>
     </row>
-    <row r="74" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="E74">
         <v>-1</v>
@@ -11931,7 +11931,7 @@
       <c r="AJ74" s="13"/>
       <c r="AR74" s="13"/>
     </row>
-    <row r="75" spans="1:44" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:44" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="E75">
         <v>-1</v>
@@ -11991,7 +11991,7 @@
       <c r="AJ75" s="13"/>
       <c r="AR75" s="13"/>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:44" x14ac:dyDescent="0.3">
       <c r="E76">
         <v>-1</v>
       </c>
@@ -12044,7 +12044,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:44" x14ac:dyDescent="0.3">
       <c r="E77">
         <v>-1</v>
       </c>
@@ -12097,7 +12097,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:44" x14ac:dyDescent="0.3">
       <c r="E78">
         <v>-1</v>
       </c>
@@ -12150,7 +12150,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:44" x14ac:dyDescent="0.3">
       <c r="E79">
         <v>-1</v>
       </c>
@@ -12203,7 +12203,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:44" x14ac:dyDescent="0.3">
       <c r="E80">
         <v>-1</v>
       </c>
@@ -12256,7 +12256,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="81" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="81" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E81">
         <v>-1</v>
       </c>
@@ -12309,7 +12309,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="82" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="82" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E82">
         <v>-1</v>
       </c>
@@ -12362,7 +12362,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="83" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="83" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E83">
         <v>-1</v>
       </c>
@@ -12415,7 +12415,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="84" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="84" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E84">
         <v>-1</v>
       </c>
@@ -12468,7 +12468,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="85" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E85">
         <v>-1</v>
       </c>
@@ -12521,7 +12521,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="86" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E86">
         <v>-1</v>
       </c>
@@ -12574,7 +12574,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="87" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="87" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E87">
         <v>-1</v>
       </c>
@@ -12627,7 +12627,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="88" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E88">
         <v>-1</v>
       </c>
@@ -12680,7 +12680,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="89" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="89" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E89">
         <v>-1</v>
       </c>
@@ -12733,7 +12733,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="90" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="90" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E90">
         <v>-1</v>
       </c>
@@ -12786,7 +12786,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="91" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="91" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E91">
         <v>-1</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="92" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E92">
         <v>-1</v>
       </c>
@@ -12892,7 +12892,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="93" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="93" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E93">
         <v>-1</v>
       </c>
@@ -12945,7 +12945,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="94" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="94" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E94">
         <v>-1</v>
       </c>
@@ -12998,7 +12998,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="95" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="95" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E95">
         <v>-1</v>
       </c>
@@ -13051,7 +13051,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="96" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="96" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E96">
         <v>-1</v>
       </c>
@@ -13104,7 +13104,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="97" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="97" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E97">
         <v>-1</v>
       </c>
@@ -13157,7 +13157,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="98" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="98" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E98">
         <v>-1</v>
       </c>
@@ -13210,7 +13210,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="99" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="99" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E99">
         <v>-1</v>
       </c>
@@ -13263,7 +13263,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="100" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="100" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E100">
         <v>-1</v>
       </c>
@@ -13316,7 +13316,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="101" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="101" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E101">
         <v>-1</v>
       </c>
@@ -13369,7 +13369,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="102" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="102" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E102">
         <v>-1</v>
       </c>
@@ -13422,7 +13422,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="103" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="103" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E103">
         <v>-1</v>
       </c>
@@ -13475,7 +13475,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="104" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="104" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E104">
         <v>-1</v>
       </c>
@@ -13528,7 +13528,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="105" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="105" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E105">
         <v>-1</v>
       </c>
@@ -13581,7 +13581,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="106" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="106" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E106">
         <v>-1</v>
       </c>
@@ -13634,7 +13634,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="107" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="107" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E107">
         <v>-1</v>
       </c>
@@ -13687,7 +13687,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="108" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="108" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E108">
         <v>-1</v>
       </c>
@@ -13740,7 +13740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="109" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="109" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E109">
         <v>-1</v>
       </c>
@@ -13793,7 +13793,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="110" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="110" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E110">
         <v>-1</v>
       </c>
@@ -13846,7 +13846,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="111" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="111" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E111">
         <v>-1</v>
       </c>
@@ -13899,7 +13899,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="112" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="112" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E112">
         <v>-1</v>
       </c>
@@ -13952,7 +13952,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="113" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="113" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E113">
         <v>-1</v>
       </c>
@@ -14005,7 +14005,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="114" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="114" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E114">
         <v>-1</v>
       </c>
@@ -14058,7 +14058,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="115" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="115" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E115">
         <v>-1</v>
       </c>
@@ -14111,7 +14111,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="116" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="116" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E116">
         <v>-1</v>
       </c>
@@ -14164,7 +14164,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="117" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="117" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E117">
         <v>-1</v>
       </c>
@@ -14217,7 +14217,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="118" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="118" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E118">
         <v>-1</v>
       </c>
@@ -14270,7 +14270,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="119" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="119" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E119">
         <v>-1</v>
       </c>
@@ -14323,7 +14323,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="120" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="120" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E120">
         <v>-1</v>
       </c>
@@ -14376,7 +14376,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="121" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="121" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E121">
         <v>-1</v>
       </c>
@@ -14429,7 +14429,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="122" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="122" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E122">
         <v>-1</v>
       </c>
@@ -14482,7 +14482,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="123" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="123" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E123">
         <v>-1</v>
       </c>
@@ -14535,7 +14535,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="124" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="124" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E124">
         <v>-1</v>
       </c>
@@ -14588,7 +14588,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="125" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="125" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E125">
         <v>-1</v>
       </c>
@@ -14641,7 +14641,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="126" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="126" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E126">
         <v>-1</v>
       </c>
@@ -14694,7 +14694,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="127" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="127" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E127">
         <v>-1</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="128" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="128" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E128">
         <v>-1</v>
       </c>
@@ -14800,7 +14800,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="129" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="129" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E129">
         <v>-1</v>
       </c>
@@ -14853,7 +14853,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="130" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="130" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E130">
         <v>-1</v>
       </c>
@@ -14906,7 +14906,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="131" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="131" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E131">
         <v>-1</v>
       </c>
@@ -14959,7 +14959,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="132" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="132" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E132">
         <v>-1</v>
       </c>
@@ -15012,7 +15012,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="133" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="133" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E133">
         <v>-1</v>
       </c>
@@ -15065,7 +15065,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="134" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="134" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E134">
         <v>-1</v>
       </c>
@@ -15118,7 +15118,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="135" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="135" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E135">
         <v>-1</v>
       </c>
@@ -15171,7 +15171,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="136" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="136" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E136">
         <v>-1</v>
       </c>
@@ -15224,7 +15224,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="137" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="137" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E137">
         <v>-1</v>
       </c>
@@ -15277,7 +15277,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="138" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="138" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E138">
         <v>-1</v>
       </c>
@@ -15330,7 +15330,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="139" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="139" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E139">
         <v>-1</v>
       </c>
@@ -15383,7 +15383,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="140" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="140" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E140">
         <v>-1</v>
       </c>
@@ -15436,7 +15436,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="141" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="141" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E141">
         <v>-1</v>
       </c>
@@ -15489,7 +15489,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="142" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="142" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E142">
         <v>-1</v>
       </c>
@@ -15542,7 +15542,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="143" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="143" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E143">
         <v>-1</v>
       </c>
@@ -15595,7 +15595,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="144" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="144" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E144">
         <v>-1</v>
       </c>
@@ -15648,7 +15648,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="145" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="145" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E145">
         <v>-1</v>
       </c>
@@ -15701,7 +15701,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="146" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="146" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E146">
         <v>-1</v>
       </c>
@@ -15754,7 +15754,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="147" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="147" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E147">
         <v>-1</v>
       </c>
@@ -15807,7 +15807,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="148" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="148" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E148">
         <v>-1</v>
       </c>
@@ -15860,7 +15860,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="149" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="149" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E149">
         <v>-1</v>
       </c>
@@ -15913,7 +15913,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="150" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="150" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E150">
         <v>-1</v>
       </c>
@@ -15966,7 +15966,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="151" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="151" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E151">
         <v>-1</v>
       </c>
@@ -16019,7 +16019,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="152" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="152" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E152">
         <v>-1</v>
       </c>
@@ -16072,7 +16072,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="153" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="153" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E153">
         <v>-1</v>
       </c>
@@ -16125,7 +16125,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="154" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="154" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E154">
         <v>-1</v>
       </c>
@@ -16178,7 +16178,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="155" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E155">
         <v>-1</v>
       </c>
@@ -16231,7 +16231,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="156" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="156" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E156">
         <v>-1</v>
       </c>
@@ -16284,7 +16284,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="157" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="157" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E157">
         <v>-1</v>
       </c>
@@ -16337,7 +16337,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="158" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="158" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E158">
         <v>-1</v>
       </c>
@@ -16390,7 +16390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="159" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="159" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E159">
         <v>-1</v>
       </c>
@@ -16443,7 +16443,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="160" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="160" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E160">
         <v>-1</v>
       </c>
@@ -16496,7 +16496,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="161" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="161" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E161">
         <v>-1</v>
       </c>
@@ -16549,7 +16549,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="162" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="162" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E162">
         <v>-1</v>
       </c>
@@ -16602,7 +16602,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="163" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="163" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E163">
         <v>-1</v>
       </c>
@@ -16655,7 +16655,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="164" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="164" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E164">
         <v>-1</v>
       </c>
@@ -16708,7 +16708,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="165" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="165" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E165">
         <v>-1</v>
       </c>
@@ -16761,7 +16761,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="166" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="166" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E166">
         <v>-1</v>
       </c>
@@ -16814,7 +16814,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="167" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="167" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E167">
         <v>-1</v>
       </c>
@@ -16867,7 +16867,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="168" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="168" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E168">
         <v>-1</v>
       </c>
@@ -16920,7 +16920,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="169" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="169" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E169">
         <v>-1</v>
       </c>
@@ -16973,7 +16973,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="170" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="170" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E170">
         <v>-1</v>
       </c>
@@ -17026,7 +17026,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="171" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="171" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E171">
         <v>-1</v>
       </c>
@@ -17079,7 +17079,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="172" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="172" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E172">
         <v>-1</v>
       </c>
@@ -17132,7 +17132,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="173" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="173" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E173">
         <v>-1</v>
       </c>
@@ -17185,7 +17185,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="174" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="174" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E174">
         <v>-1</v>
       </c>
@@ -17238,7 +17238,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="175" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="175" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E175">
         <v>-1</v>
       </c>
@@ -17291,7 +17291,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="176" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="176" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E176">
         <v>-1</v>
       </c>
@@ -17344,7 +17344,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="177" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="177" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E177">
         <v>-1</v>
       </c>
@@ -17397,7 +17397,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="178" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="178" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E178">
         <v>-1</v>
       </c>
@@ -17450,7 +17450,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="179" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="179" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E179">
         <v>-1</v>
       </c>
@@ -17503,7 +17503,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="180" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="180" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E180">
         <v>-1</v>
       </c>
@@ -17556,7 +17556,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="181" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="181" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E181">
         <v>-1</v>
       </c>
@@ -17609,7 +17609,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="182" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="182" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E182">
         <v>-1</v>
       </c>
@@ -17662,7 +17662,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="183" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="183" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E183">
         <v>-1</v>
       </c>
@@ -17715,7 +17715,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="184" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="184" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E184">
         <v>-1</v>
       </c>
@@ -17768,7 +17768,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="185" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="185" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E185">
         <v>-1</v>
       </c>
@@ -17821,7 +17821,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="186" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="186" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E186">
         <v>-1</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="187" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="187" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E187">
         <v>-1</v>
       </c>
@@ -17927,7 +17927,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="188" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="188" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E188">
         <v>-1</v>
       </c>
@@ -17980,7 +17980,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="189" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="189" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E189">
         <v>-1</v>
       </c>
@@ -18033,7 +18033,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="190" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="190" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E190">
         <v>-1</v>
       </c>
@@ -18086,7 +18086,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="191" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="191" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E191">
         <v>-1</v>
       </c>
@@ -18139,7 +18139,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="192" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="192" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E192">
         <v>-1</v>
       </c>
@@ -18192,7 +18192,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="193" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="193" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E193">
         <v>-1</v>
       </c>
@@ -18245,7 +18245,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="194" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="194" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E194">
         <v>-1</v>
       </c>
@@ -18298,7 +18298,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="195" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="195" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E195">
         <v>-1</v>
       </c>
@@ -18351,7 +18351,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="196" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="196" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E196">
         <v>-1</v>
       </c>
@@ -18404,7 +18404,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="197" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="197" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E197">
         <v>-1</v>
       </c>
@@ -18457,7 +18457,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="198" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="198" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E198">
         <v>-1</v>
       </c>
@@ -18510,7 +18510,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="199" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="199" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E199">
         <v>-1</v>
       </c>
@@ -18563,7 +18563,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="200" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="200" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E200">
         <v>-1</v>
       </c>
@@ -18616,7 +18616,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="201" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="201" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E201">
         <v>-1</v>
       </c>
@@ -18669,7 +18669,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="202" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="202" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E202">
         <v>-1</v>
       </c>
@@ -18722,7 +18722,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="203" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="203" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E203">
         <v>-1</v>
       </c>
@@ -18775,7 +18775,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="204" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="204" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E204">
         <v>-1</v>
       </c>
@@ -18828,7 +18828,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="205" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="205" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E205">
         <v>-1</v>
       </c>
@@ -18881,7 +18881,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="206" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="206" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E206">
         <v>-1</v>
       </c>
@@ -18934,7 +18934,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="207" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="207" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E207">
         <v>-1</v>
       </c>
@@ -18987,7 +18987,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="208" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="208" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E208">
         <v>-1</v>
       </c>
@@ -19040,7 +19040,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="209" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="209" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E209">
         <v>-1</v>
       </c>
@@ -19093,7 +19093,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="210" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="210" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E210">
         <v>-1</v>
       </c>
@@ -19146,7 +19146,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="211" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="211" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E211">
         <v>-1</v>
       </c>
@@ -19199,7 +19199,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="212" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="212" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E212">
         <v>-1</v>
       </c>
@@ -19252,7 +19252,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="213" spans="5:31" x14ac:dyDescent="0.5">
+    <row r="213" spans="5:31" x14ac:dyDescent="0.3">
       <c r="E213">
         <v>-1</v>
       </c>
@@ -19321,13 +19321,13 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.64453125" customWidth="1"/>
-    <col min="5" max="5" width="16.52734375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
@@ -19344,7 +19344,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -19371,16 +19371,17 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.52734375" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
@@ -19394,7 +19395,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>255</v>
       </c>
@@ -19408,7 +19409,7 @@
         <v>11920</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>279</v>
       </c>
@@ -19436,17 +19437,17 @@
       <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.52734375" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.52734375" customWidth="1"/>
-    <col min="10" max="10" width="15.3515625" customWidth="1"/>
-    <col min="11" max="11" width="15.87890625" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
     <col min="12" max="12" width="14" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -19484,7 +19485,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -19522,7 +19523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -19560,7 +19561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -19598,7 +19599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -19636,7 +19637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -19674,7 +19675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -19712,7 +19713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -19750,7 +19751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -19788,7 +19789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -19826,7 +19827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -19879,20 +19880,20 @@
       <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.41015625" customWidth="1"/>
-    <col min="2" max="2" width="14.41015625" customWidth="1"/>
-    <col min="3" max="3" width="18.52734375" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.64453125" customWidth="1"/>
-    <col min="6" max="8" width="16.52734375" customWidth="1"/>
-    <col min="12" max="13" width="8.1171875" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="8" width="16.5546875" customWidth="1"/>
+    <col min="12" max="13" width="8.109375" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
-    <col min="16" max="16" width="17.52734375" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -19984,7 +19985,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -20073,7 +20074,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -20162,7 +20163,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -20251,7 +20252,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -20340,7 +20341,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -20432,7 +20433,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -20521,32 +20522,32 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>19</v>
       </c>
@@ -20565,13 +20566,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.234375" customWidth="1"/>
-    <col min="3" max="3" width="28.52734375" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>177</v>
       </c>
@@ -20588,7 +20589,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -20605,7 +20606,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>72</v>
       </c>
@@ -20622,7 +20623,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>73</v>
       </c>
@@ -20639,7 +20640,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>74</v>
       </c>
@@ -20656,7 +20657,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>75</v>
       </c>
@@ -20673,7 +20674,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>75</v>
       </c>
@@ -20704,24 +20705,24 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.87890625" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.3515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.87890625" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1171875" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.3515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.52734375" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1171875" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1171875" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.41015625" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.52734375" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.52734375" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.87890625" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.87890625" style="24"/>
+    <col min="1" max="1" width="14.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>10</v>
       </c>
@@ -20759,7 +20760,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>232</v>
       </c>
@@ -20811,12 +20812,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.87890625" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -20863,7 +20864,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -20924,12 +20925,12 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.1171875" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -20958,7 +20959,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>179</v>
       </c>
@@ -21001,15 +21002,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.3515625" customWidth="1"/>
-    <col min="2" max="2" width="13.41015625" customWidth="1"/>
-    <col min="8" max="8" width="13.1171875" customWidth="1"/>
-    <col min="19" max="19" width="11.52734375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="19" max="19" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>177</v>
       </c>
@@ -21080,7 +21081,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>75</v>
       </c>
@@ -21151,7 +21152,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -21223,7 +21224,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>74</v>
       </c>
@@ -21294,7 +21295,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>73</v>
       </c>
@@ -21365,7 +21366,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>72</v>
       </c>
@@ -21436,19 +21437,19 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:23" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
     </row>
-    <row r="17" spans="1:1" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
     </row>
-    <row r="18" spans="1:1" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
     </row>
-    <row r="19" spans="1:1" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
     </row>
   </sheetData>
@@ -21468,16 +21469,16 @@
       <selection activeCell="E1" sqref="E1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.52734375" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="10" max="10" width="14.87890625" customWidth="1"/>
-    <col min="11" max="11" width="13.52734375" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -21515,7 +21516,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -21541,7 +21542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -21567,7 +21568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -21593,7 +21594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -21619,7 +21620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -21648,7 +21649,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -21674,7 +21675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -21700,7 +21701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -21726,7 +21727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -21752,7 +21753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -21778,7 +21779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -21804,7 +21805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -21831,7 +21832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -21857,7 +21858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -21883,7 +21884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -21912,7 +21913,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -21938,7 +21939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -21980,12 +21981,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.87890625" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -21999,7 +22000,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>271</v>
       </c>
@@ -22027,14 +22028,14 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.41015625" customWidth="1"/>
-    <col min="6" max="6" width="15.41015625" customWidth="1"/>
-    <col min="10" max="10" width="15.64453125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -22072,7 +22073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -22110,7 +22111,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -22145,7 +22146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -22180,7 +22181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -22215,7 +22216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -22250,7 +22251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -22285,7 +22286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>173</v>
       </c>
@@ -22320,7 +22321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>174</v>
       </c>
@@ -22369,13 +22370,13 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.3515625" customWidth="1"/>
-    <col min="3" max="3" width="11.64453125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -22386,7 +22387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -22397,7 +22398,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -22408,7 +22409,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -22419,7 +22420,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -22430,7 +22431,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -22441,7 +22442,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -22452,7 +22453,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -22463,7 +22464,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -22474,7 +22475,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -22485,7 +22486,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -22496,7 +22497,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -22507,7 +22508,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -22518,7 +22519,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -22529,7 +22530,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -22540,7 +22541,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -22551,7 +22552,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -22562,7 +22563,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -22573,7 +22574,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -22584,7 +22585,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -22595,7 +22596,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -22606,7 +22607,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -22617,7 +22618,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -22628,7 +22629,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -22639,7 +22640,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -22650,7 +22651,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -22661,7 +22662,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -22672,7 +22673,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -22683,7 +22684,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -22694,7 +22695,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -22705,7 +22706,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -22716,7 +22717,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -22727,7 +22728,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
@@ -22738,7 +22739,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -22749,7 +22750,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>15</v>
       </c>
@@ -22760,7 +22761,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>15</v>
       </c>
@@ -22771,7 +22772,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>15</v>
       </c>
@@ -22782,7 +22783,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
@@ -22793,7 +22794,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>15</v>
       </c>
@@ -22804,7 +22805,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
@@ -22815,7 +22816,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>15</v>
       </c>
@@ -22826,7 +22827,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>15</v>
       </c>
@@ -22837,7 +22838,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>15</v>
       </c>
@@ -22848,7 +22849,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>15</v>
       </c>
@@ -22859,7 +22860,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>15</v>
       </c>
@@ -22870,7 +22871,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>15</v>
       </c>
@@ -22881,7 +22882,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>15</v>
       </c>
@@ -22892,7 +22893,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>15</v>
       </c>
@@ -22903,7 +22904,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>15</v>
       </c>
@@ -22914,7 +22915,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>16</v>
       </c>
@@ -22925,7 +22926,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -22936,7 +22937,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -22947,7 +22948,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -22958,7 +22959,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -22969,7 +22970,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>16</v>
       </c>
@@ -22980,7 +22981,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>16</v>
       </c>
@@ -22991,7 +22992,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>16</v>
       </c>
@@ -23002,7 +23003,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>16</v>
       </c>
@@ -23013,7 +23014,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>16</v>
       </c>
@@ -23024,7 +23025,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>16</v>
       </c>
@@ -23035,7 +23036,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>16</v>
       </c>
@@ -23046,7 +23047,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>16</v>
       </c>
@@ -23057,7 +23058,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>16</v>
       </c>
@@ -23068,7 +23069,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>16</v>
       </c>
@@ -23079,7 +23080,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>16</v>
       </c>
@@ -23090,7 +23091,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>16</v>
       </c>
@@ -23101,7 +23102,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>16</v>
       </c>
@@ -23112,7 +23113,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>16</v>
       </c>
@@ -23123,21 +23124,21 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
     </row>
-    <row r="70" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
     </row>
-    <row r="71" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>19</v>
       </c>
@@ -23148,7 +23149,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>19</v>
       </c>
@@ -23159,7 +23160,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>20</v>
       </c>
@@ -23170,7 +23171,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>20</v>
       </c>
@@ -23181,7 +23182,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>20</v>
       </c>
@@ -23192,7 +23193,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>20</v>
       </c>
@@ -23203,7 +23204,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>20</v>
       </c>
@@ -23214,7 +23215,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -23225,7 +23226,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>21</v>
       </c>
@@ -23236,7 +23237,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -23247,7 +23248,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -23258,7 +23259,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -23269,7 +23270,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -23280,7 +23281,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>22</v>
       </c>
@@ -23291,7 +23292,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>22</v>
       </c>
@@ -23302,7 +23303,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>22</v>
       </c>
@@ -23313,7 +23314,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>22</v>
       </c>
@@ -23339,9 +23340,9 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -23375,9 +23376,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -23388,210 +23389,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086EABF47CD1113448A96A17F6C8D13F9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c68283fca48dae9b1add248de89d15c2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a5f42ec3-4ee2-45fc-8d77-288bf2f0f986" xmlns:ns3="73fb875a-8af9-4255-b008-0995492d31cd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40d2b883f32ec076906f2da59f0ebb5f" ns2:_="" ns3:_="">
-    <xsd:import namespace="a5f42ec3-4ee2-45fc-8d77-288bf2f0f986"/>
-    <xsd:import namespace="73fb875a-8af9-4255-b008-0995492d31cd"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a5f42ec3-4ee2-45fc-8d77-288bf2f0f986" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="8ff62593-b918-4deb-ac08-0d74ac0cc7e6" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="73fb875a-8af9-4255-b008-0995492d31cd" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="17" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{77211ec7-9289-48e1-8a25-db087204c2aa}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="442dd8d0-93bc-4a15-a2cd-49423a906912">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4062F44-2271-442E-A9E4-C9D848982103}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DDECB4A-9ABF-4708-96AE-8CBC59050E2E}"/>
 </file>
</xml_diff>

<commit_message>
Updated input excel data for irrigation
</commit_message>
<xml_diff>
--- a/Example input/Kansas/kansas inputs.xlsx
+++ b/Example input/Kansas/kansas inputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2283CF0A-204F-4581-A05F-2ACF2463BF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683E75D6-A396-43E4-B7AB-BD49EDC32808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="852" windowWidth="17988" windowHeight="11652" tabRatio="824" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23508" yWindow="1476" windowWidth="17280" windowHeight="9072" tabRatio="824" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="5" r:id="rId1"/>
@@ -14,18 +14,19 @@
     <sheet name="Fertilization" sheetId="1" r:id="rId4"/>
     <sheet name="Tillage" sheetId="21" r:id="rId5"/>
     <sheet name="GridRatio" sheetId="11" r:id="rId6"/>
-    <sheet name="Irrig" sheetId="3" r:id="rId7"/>
-    <sheet name="Drip" sheetId="16" r:id="rId8"/>
-    <sheet name="DripNodes" sheetId="17" r:id="rId9"/>
-    <sheet name="Init" sheetId="2" r:id="rId10"/>
-    <sheet name="Soil" sheetId="6" r:id="rId11"/>
-    <sheet name="Solute" sheetId="15" r:id="rId12"/>
-    <sheet name="Gas" sheetId="19" r:id="rId13"/>
-    <sheet name="Time" sheetId="4" r:id="rId14"/>
-    <sheet name="Variety" sheetId="10" r:id="rId15"/>
-    <sheet name="Weather" sheetId="7" r:id="rId16"/>
-    <sheet name="MulchDecomp" sheetId="18" r:id="rId17"/>
-    <sheet name="MulchGeo" sheetId="20" r:id="rId18"/>
+    <sheet name="Irrig_data" sheetId="3" r:id="rId7"/>
+    <sheet name="Irrig" sheetId="22" r:id="rId8"/>
+    <sheet name="Drip" sheetId="16" r:id="rId9"/>
+    <sheet name="DripNodes" sheetId="17" r:id="rId10"/>
+    <sheet name="Init" sheetId="2" r:id="rId11"/>
+    <sheet name="Soil" sheetId="6" r:id="rId12"/>
+    <sheet name="Solute" sheetId="15" r:id="rId13"/>
+    <sheet name="Gas" sheetId="19" r:id="rId14"/>
+    <sheet name="Time" sheetId="4" r:id="rId15"/>
+    <sheet name="Variety" sheetId="10" r:id="rId16"/>
+    <sheet name="Weather" sheetId="7" r:id="rId17"/>
+    <sheet name="MulchDecomp" sheetId="18" r:id="rId18"/>
+    <sheet name="MulchGeo" sheetId="20" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -270,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="296">
   <si>
     <t>Date</t>
   </si>
@@ -1155,6 +1156,9 @@
   </si>
   <si>
     <t>seedDepth</t>
+  </si>
+  <si>
+    <t>amount (mm/day)</t>
   </si>
 </sst>
 </file>
@@ -1406,9 +1410,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1446,9 +1450,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1481,26 +1485,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1533,26 +1520,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2455,12 +2425,36 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EC46E5-4664-4FE7-A277-7DF4620FA352}">
+  <sheetPr codeName="Sheet15"/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2539,7 +2533,7 @@
         <v>19</v>
       </c>
       <c r="B2">
-        <v>69167</v>
+        <v>68000</v>
       </c>
       <c r="C2">
         <v>39.130000000000003</v>
@@ -2651,7 +2645,7 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>66900</v>
+        <v>68000</v>
       </c>
       <c r="C4">
         <v>39.130000000000003</v>
@@ -3104,7 +3098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AR213"/>
@@ -19312,7 +19306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:E2"/>
@@ -19366,12 +19360,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558FADBF-76C4-4D91-8CE7-6DF079B1F138}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -19428,7 +19422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:L11"/>
@@ -19871,7 +19865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AD17"/>
@@ -20557,7 +20551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:E7"/>
@@ -20696,7 +20690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9600C260-045B-494F-96B8-C4B2D07CC3E3}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:L2"/>
@@ -20803,7 +20797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39CF59C2-B851-4956-A7BA-5B8FBABCF390}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:O2"/>
@@ -21465,8 +21459,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22367,7 +22361,7 @@
   <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22384,7 +22378,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>1</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -23332,6 +23326,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2162BF-70BD-4136-A395-41A98066B4E6}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F5D1D0-E783-4E15-BB8E-68B8E93C0057}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:F1"/>
@@ -23365,28 +23386,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EC46E5-4664-4FE7-A277-7DF4620FA352}">
-  <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>